<commit_message>
Age Photo Exp Finished
</commit_message>
<xml_diff>
--- a/age_gender/performance.xlsx
+++ b/age_gender/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="5880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="252">
   <si>
     <t>FGNET</t>
   </si>
@@ -758,6 +758,21 @@
   </si>
   <si>
     <t>Feature HOG 6 orient</t>
+  </si>
+  <si>
+    <t>Align 2.1</t>
+  </si>
+  <si>
+    <t>Align 2.2</t>
+  </si>
+  <si>
+    <t>Align l2</t>
+  </si>
+  <si>
+    <t>Align l1</t>
+  </si>
+  <si>
+    <t>Align l0</t>
   </si>
 </sst>
 </file>
@@ -2840,10 +2855,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2856,7 +2871,7 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>246</v>
       </c>
@@ -2876,7 +2891,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -2893,7 +2908,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -2901,54 +2916,75 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="B15">
+        <v>5.004651</v>
+      </c>
+      <c r="C15">
+        <v>11.678654999999999</v>
+      </c>
+      <c r="D15">
+        <v>11.845544</v>
+      </c>
+      <c r="I15" t="s">
+        <v>247</v>
+      </c>
+      <c r="J15">
+        <v>5.1379999999999999</v>
+      </c>
+      <c r="K15">
+        <v>9.5967000000000002</v>
+      </c>
+      <c r="L15">
+        <v>12.128399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>250</v>
       </c>
       <c r="B16">
         <v>4.0962740000000002</v>
@@ -2959,58 +2995,116 @@
       <c r="D16">
         <v>10.179871</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>248</v>
+      </c>
+      <c r="J16">
+        <v>4.1007999999999996</v>
+      </c>
+      <c r="K16">
+        <v>7.0898000000000003</v>
+      </c>
+      <c r="L16">
+        <v>10.397500000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+        <v>249</v>
+      </c>
+      <c r="B17">
+        <v>3.8642110000000001</v>
+      </c>
+      <c r="C17">
+        <v>6.7567539999999999</v>
+      </c>
+      <c r="D17">
+        <v>9.9262250000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>247</v>
+      </c>
+      <c r="J19">
+        <v>0.57820000000000005</v>
+      </c>
+      <c r="K19">
+        <v>0.34360000000000002</v>
+      </c>
+      <c r="L19">
+        <v>0.31059999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>251</v>
+      </c>
+      <c r="B22">
+        <v>0.58441600000000005</v>
+      </c>
+      <c r="C22">
+        <v>0.28919499999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.31924000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B23">
+        <v>0.680064</v>
+      </c>
+      <c r="C23">
+        <v>0.44700400000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.36642599999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>249</v>
+      </c>
+      <c r="B24">
+        <v>0.71096400000000004</v>
+      </c>
+      <c r="C24">
+        <v>0.47380499999999998</v>
+      </c>
+      <c r="D24">
+        <v>0.37480599999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>230</v>
       </c>
-      <c r="B21">
-        <v>0.680064</v>
-      </c>
-      <c r="C21">
-        <v>0.44700400000000001</v>
-      </c>
-      <c r="D21">
-        <v>0.36642599999999997</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>231</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Age Exp Refined. OpenMP added to feature
</commit_message>
<xml_diff>
--- a/age_gender/performance.xlsx
+++ b/age_gender/performance.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="5880" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="5880" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="394">
   <si>
     <t>FGNET</t>
   </si>
@@ -757,15 +759,6 @@
     <t>7779/8000</t>
   </si>
   <si>
-    <t>Feature HOG 6 orient</t>
-  </si>
-  <si>
-    <t>Align 2.1</t>
-  </si>
-  <si>
-    <t>Align 2.2</t>
-  </si>
-  <si>
     <t>Align l2</t>
   </si>
   <si>
@@ -773,6 +766,441 @@
   </si>
   <si>
     <t>Align l0</t>
+  </si>
+  <si>
+    <t>Feature HOG 8 orient 0.5/0.5</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>Train on WebFace, Test on WebFace</t>
+  </si>
+  <si>
+    <t>Train on Yamaha, Test on Yamaha</t>
+  </si>
+  <si>
+    <t>Train on Morph2, Test on Morph2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Split Acc=0.777646, MAE=4.737304, AgeACC=0.643221, GenderACC=0.955364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    4.6745    0.6474    0.9586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    5.6194    0.5838    0.9099</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0   10.1279    0.2917    0.6250</t>
+  </si>
+  <si>
+    <t>Split Acc=0.708804, MAE=6.236441, AgeACC=0.632993, GenderACC=0.893322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    5.8216    0.6531    0.8575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    7.1550    0.5822    0.8290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0   12.8751    0.4280    0.7627</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Split Acc=0.833192, MAE=3.678508, AgeACC=0.750322, GenderACC=0.979272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    3.6424    0.7538    0.9807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    4.1825    0.7016    0.9584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    6.3046    0.5208    0.9375</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Split Acc=0.659148, MAE=7.105751, AgeACC=0.562263, GenderACC=0.862581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    6.8218    0.5760    0.8189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0    7.8201    0.5253    0.7906</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         0   10.2947    0.4479    0.7838</t>
+  </si>
+  <si>
+    <t>View 1</t>
+  </si>
+  <si>
+    <t>View 2</t>
+  </si>
+  <si>
+    <t>View 3</t>
+  </si>
+  <si>
+    <t>View 4</t>
+  </si>
+  <si>
+    <t>Split Acc</t>
+  </si>
+  <si>
+    <t>Age Acc</t>
+  </si>
+  <si>
+    <t>Gender Acc</t>
+  </si>
+  <si>
+    <t>Overall</t>
+  </si>
+  <si>
+    <t>Align Lv0</t>
+  </si>
+  <si>
+    <t>Align Lv1</t>
+  </si>
+  <si>
+    <t>Align Lv2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> split acc </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MAE </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> age acc </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gender acc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7257    5.4650    0.5750    0.9375</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7299    5.4053    0.5780    0.9407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6693    6.2602    0.5345    0.8920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.4938    9.9461    0.3688    0.8063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6594    7.7447    0.5378    0.8703</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6697    7.2597    0.5539    0.8775</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6383    8.7709    0.5050    0.8524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5452   12.8573    0.3564    0.8202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5004   11.9436    0.4057    0.7265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5025   11.6512    0.4235    0.7171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5010   12.2384    0.3838    0.7434</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.4513   14.3309    0.3076    0.7051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.2167   19.6779    0.2833    0.3833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7771    4.7169    0.6446    0.9517</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7823    4.6456    0.6492    0.9553</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7072    5.6552    0.5824    0.9025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.4437   10.6763    0.3312    0.7063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7099    6.0929    0.6461    0.8756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7217    5.6272    0.6686    0.8814</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6881    6.9151    0.5938    0.8695</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5543   12.5977    0.4585    0.7535</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5256   10.9276    0.4300    0.7534</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5335   10.4289    0.4548    0.7510</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5193   11.4867    0.3997    0.7597</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.4388   14.2855    0.2897    0.7252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.2833   21.4668    0.2000    0.5500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7749    4.0157    0.7211    0.9649</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7783    3.9686    0.7251    0.9668</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.7307    4.6408    0.6675    0.9379</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5000    7.6393    0.4250    0.8750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6139    7.8816    0.5509    0.8204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6155    7.5951    0.5648    0.8227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.6159    8.3139    0.5201    0.8187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5458   12.6182    0.4189    0.7669</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5055   10.6950    0.4918    0.7432</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5086   10.3473    0.5099    0.7415</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5056   11.0539    0.4717    0.7489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.4334   13.6434    0.3606    0.7062</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.5500   11.5775    0.3000    0.7167</t>
+  </si>
+  <si>
+    <t>fold 1,fold 2,fold 3,fold 4,fold 5,fold 6,fold 7,fold 8,fold 9,fold 10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    9.8770    0.3384         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    9.5054    0.3499         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000   10.7958    0.3093         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000   12.4212    0.2667         0</t>
+  </si>
+  <si>
+    <t>align_name =</t>
+  </si>
+  <si>
+    <t>AlignLv1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    8.1235    0.4097         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    7.8056    0.4221         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    8.8543    0.3817         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000   10.8776    0.2982         0</t>
+  </si>
+  <si>
+    <t>AlignLv2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    6.3731    0.4965         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    6.1198    0.5124         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    6.9668    0.4603         0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1.0000    8.4480    0.3567         0</t>
+  </si>
+  <si>
+    <t>AlignLv0</t>
+  </si>
+  <si>
+    <t>fold 1,3   if ~isempty(model_path)</t>
+  </si>
+  <si>
+    <t>fold 2,fold 3,fold 4,fold 5,fold 6,fold 7,fold 8,fold 9,fold 10,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.9142    0.3336    0.8446</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.5584    0.3398    0.8502</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.7594    0.3183    0.8312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.7267    0.2933    0.8002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8.0936    0.4087    0.8978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7.8467    0.4160    0.9086</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8.6275    0.3940    0.8763</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.5522    0.3244    0.7721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.7141    0.6145    0.9631</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.6631    0.6189    0.9659</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5.4117    0.5524    0.9242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7.5701    0.4375    0.8063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.2241    0.6695    0.9705</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.1688    0.6745    0.9732</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.9707    0.6003    0.9372</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7.8524    0.4750    0.5938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11.0353    0.3207    0.8001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.8119    0.3317    0.8026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11.1124    0.3136    0.8048</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.0057    0.2841    0.7645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   15.7863    0.2295    0.6627</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.8406    0.3253    0.7978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.5267    0.3386    0.8025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.9206    0.3185    0.8028</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.4097    0.2727    0.7494</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   16.7941    0.1820    0.6153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.5471    0.4789    0.9076</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.3361    0.4899    0.9111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7.0334    0.4516    0.8927</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8.3539    0.4040    0.9464</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.0068    0.6905    0.9672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.9730    0.6943    0.9688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4.4646    0.6396    0.9458</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6.1163    0.4562    0.8750</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.0031    0.3475    0.8484</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.9696    0.3504    0.8468</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.8863    0.3519    0.8548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.6817    0.3104    0.8364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   14.2773    0.1738    0.6475</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11.0212    0.3210    0.8081</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.8178    0.3325    0.8087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   11.0738    0.3145    0.8158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.2069    0.2730    0.7643</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.8240    0.3267    0.8079</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.5100    0.3408    0.8123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.9383    0.3180    0.8128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   12.4725    0.2718    0.7530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.9632    0.3492    0.8481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.9322    0.3510    0.8448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.8996    0.3531    0.8554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   10.5405    0.3140    0.8322</t>
   </si>
 </sst>
 </file>
@@ -811,7 +1239,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -834,11 +1262,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -857,11 +1365,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,13 +1715,13 @@
       <c r="B4" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -1736,56 +2263,56 @@
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
-      <c r="C30" s="9"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
       <c r="D31" s="6"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="6"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
       <c r="D33" s="6"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-      <c r="C35" s="9"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
@@ -2855,10 +3382,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,9 +3398,9 @@
     <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
@@ -2890,8 +3417,29 @@
       <c r="G1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>229</v>
+      </c>
+      <c r="J1" t="s">
+        <v>230</v>
+      </c>
+      <c r="K1" t="s">
+        <v>231</v>
+      </c>
+      <c r="M1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O1" t="s">
+        <v>229</v>
+      </c>
+      <c r="P1" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>238</v>
       </c>
@@ -2908,7 +3456,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>240</v>
       </c>
@@ -2916,49 +3464,93 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>5.0823999999999998</v>
+      </c>
+      <c r="J13">
+        <v>4.0529000000000002</v>
+      </c>
+      <c r="K13">
+        <v>3.8218999999999999</v>
+      </c>
+      <c r="O13">
+        <v>5.0823999999999998</v>
+      </c>
+      <c r="P13">
+        <v>4.0529000000000002</v>
+      </c>
+      <c r="Q13">
+        <v>3.8218999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>5.7542</v>
+      </c>
+      <c r="J14">
+        <v>4.7184999999999997</v>
+      </c>
+      <c r="K14">
+        <v>4.4438000000000004</v>
+      </c>
+      <c r="O14">
+        <v>5.7542</v>
+      </c>
+      <c r="P14">
+        <v>4.7184999999999997</v>
+      </c>
+      <c r="Q14">
+        <v>4.4438000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B15">
         <v>5.004651</v>
@@ -2969,22 +3561,28 @@
       <c r="D15">
         <v>11.845544</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15">
+        <v>7.0956999999999999</v>
+      </c>
+      <c r="J15">
+        <v>8.8888999999999996</v>
+      </c>
+      <c r="K15">
+        <v>7.8966000000000003</v>
+      </c>
+      <c r="O15">
+        <v>7.0956999999999999</v>
+      </c>
+      <c r="P15">
+        <v>8.8888999999999996</v>
+      </c>
+      <c r="Q15">
+        <v>7.8966000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>247</v>
-      </c>
-      <c r="J15">
-        <v>5.1379999999999999</v>
-      </c>
-      <c r="K15">
-        <v>9.5967000000000002</v>
-      </c>
-      <c r="L15">
-        <v>12.128399999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>250</v>
       </c>
       <c r="B16">
         <v>4.0962740000000002</v>
@@ -2995,22 +3593,10 @@
       <c r="D16">
         <v>10.179871</v>
       </c>
-      <c r="I16" t="s">
-        <v>248</v>
-      </c>
-      <c r="J16">
-        <v>4.1007999999999996</v>
-      </c>
-      <c r="K16">
-        <v>7.0898000000000003</v>
-      </c>
-      <c r="L16">
-        <v>10.397500000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B17">
         <v>3.8642110000000001</v>
@@ -3022,94 +3608,1941 @@
         <v>9.9262250000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I19" t="s">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="I18">
+        <v>0.58209999999999995</v>
+      </c>
+      <c r="J18">
+        <v>0.68520000000000003</v>
+      </c>
+      <c r="K18">
+        <v>0.71660000000000001</v>
+      </c>
+      <c r="O18">
+        <v>0.58209999999999995</v>
+      </c>
+      <c r="P18">
+        <v>0.68520000000000003</v>
+      </c>
+      <c r="Q18">
+        <v>0.71660000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>203</v>
+      </c>
+      <c r="I19">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="J19">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="K19">
+        <v>0.64219999999999999</v>
+      </c>
+      <c r="O19">
+        <v>0.53010000000000002</v>
+      </c>
+      <c r="P19">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="Q19">
+        <v>0.64219999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>248</v>
+      </c>
+      <c r="B20">
+        <v>0.58441600000000005</v>
+      </c>
+      <c r="C20">
+        <v>0.28919499999999998</v>
+      </c>
+      <c r="D20">
+        <v>0.31924000000000002</v>
+      </c>
+      <c r="I20">
+        <v>0.45</v>
+      </c>
+      <c r="J20">
+        <v>0.33019999999999999</v>
+      </c>
+      <c r="K20">
+        <v>0.2737</v>
+      </c>
+      <c r="O20">
+        <v>0.45</v>
+      </c>
+      <c r="P20">
+        <v>0.33019999999999999</v>
+      </c>
+      <c r="Q20">
+        <v>0.2737</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>247</v>
       </c>
-      <c r="J19">
-        <v>0.57820000000000005</v>
-      </c>
-      <c r="K19">
-        <v>0.34360000000000002</v>
-      </c>
-      <c r="L19">
-        <v>0.31059999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="I20" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0.680064</v>
+      </c>
+      <c r="C21">
+        <v>0.44700400000000001</v>
+      </c>
+      <c r="D21">
+        <v>0.36642599999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="B22">
-        <v>0.58441600000000005</v>
+        <v>0.71096400000000004</v>
       </c>
       <c r="C22">
-        <v>0.28919499999999998</v>
+        <v>0.47380499999999998</v>
       </c>
       <c r="D22">
-        <v>0.31924000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>250</v>
-      </c>
-      <c r="B23">
-        <v>0.680064</v>
-      </c>
-      <c r="C23">
-        <v>0.44700400000000001</v>
-      </c>
-      <c r="D23">
-        <v>0.36642599999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>0.37480599999999997</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="I23">
+        <v>9.2802000000000007</v>
+      </c>
+      <c r="J23">
+        <v>6.7407000000000004</v>
+      </c>
+      <c r="K23">
+        <v>6.4721000000000002</v>
+      </c>
+      <c r="O23">
+        <v>9.2802000000000007</v>
+      </c>
+      <c r="P23">
+        <v>6.7407000000000004</v>
+      </c>
+      <c r="Q23">
+        <v>6.4721000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>249</v>
-      </c>
-      <c r="B24">
-        <v>0.71096400000000004</v>
-      </c>
-      <c r="C24">
-        <v>0.47380499999999998</v>
-      </c>
-      <c r="D24">
-        <v>0.37480599999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="I24">
+        <v>10.4505</v>
+      </c>
+      <c r="J24">
+        <v>7.8036000000000003</v>
+      </c>
+      <c r="K24">
+        <v>7.2714999999999996</v>
+      </c>
+      <c r="O24">
+        <v>10.4505</v>
+      </c>
+      <c r="P24">
+        <v>7.8036000000000003</v>
+      </c>
+      <c r="Q24">
+        <v>7.2714999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="I25">
+        <v>12.073</v>
+      </c>
+      <c r="J25">
+        <v>10.1829</v>
+      </c>
+      <c r="K25">
+        <v>8.7472999999999992</v>
+      </c>
+      <c r="O25">
+        <v>12.073</v>
+      </c>
+      <c r="P25">
+        <v>10.1829</v>
+      </c>
+      <c r="Q25">
+        <v>8.7472999999999992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="I26">
+        <v>30.012899999999998</v>
+      </c>
+      <c r="J26">
+        <v>17.271699999999999</v>
+      </c>
+      <c r="K26">
+        <v>9.9297000000000004</v>
+      </c>
+      <c r="O26">
+        <v>30.012899999999998</v>
+      </c>
+      <c r="P26">
+        <v>17.271699999999999</v>
+      </c>
+      <c r="Q26">
+        <v>9.9297000000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>0.3473</v>
+      </c>
+      <c r="J28">
+        <v>0.46579999999999999</v>
+      </c>
+      <c r="K28">
+        <v>0.49020000000000002</v>
+      </c>
+      <c r="O28">
+        <v>0.3473</v>
+      </c>
+      <c r="P28">
+        <v>0.46579999999999999</v>
+      </c>
+      <c r="Q28">
+        <v>0.49020000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>0.32179999999999997</v>
+      </c>
+      <c r="J29">
+        <v>0.41749999999999998</v>
+      </c>
+      <c r="K29">
+        <v>0.44490000000000002</v>
+      </c>
+      <c r="O29">
+        <v>0.32179999999999997</v>
+      </c>
+      <c r="P29">
+        <v>0.41749999999999998</v>
+      </c>
+      <c r="Q29">
+        <v>0.44490000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
+      <c r="I30">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="J30">
+        <v>0.28029999999999999</v>
+      </c>
+      <c r="K30">
+        <v>0.41270000000000001</v>
+      </c>
+      <c r="O30">
+        <v>0.27660000000000001</v>
+      </c>
+      <c r="P30">
+        <v>0.28029999999999999</v>
+      </c>
+      <c r="Q30">
+        <v>0.41270000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0.2</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+      <c r="H32" t="s">
+        <v>32</v>
+      </c>
+      <c r="N32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="I33">
+        <v>11.7895</v>
+      </c>
+      <c r="J33">
+        <v>9.7744999999999997</v>
+      </c>
+      <c r="K33">
+        <v>9.6369000000000007</v>
+      </c>
+      <c r="O33">
+        <v>11.7895</v>
+      </c>
+      <c r="P33">
+        <v>9.7744999999999997</v>
+      </c>
+      <c r="Q33">
+        <v>9.6369000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
+      <c r="I34">
+        <v>12.2372</v>
+      </c>
+      <c r="J34">
+        <v>10.383100000000001</v>
+      </c>
+      <c r="K34">
+        <v>10.0937</v>
+      </c>
+      <c r="O34">
+        <v>12.2372</v>
+      </c>
+      <c r="P34">
+        <v>10.383100000000001</v>
+      </c>
+      <c r="Q34">
+        <v>10.0937</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="I35">
+        <v>13.6455</v>
+      </c>
+      <c r="J35">
+        <v>11.8538</v>
+      </c>
+      <c r="K35">
+        <v>11.264699999999999</v>
+      </c>
+      <c r="O35">
+        <v>13.6455</v>
+      </c>
+      <c r="P35">
+        <v>11.8538</v>
+      </c>
+      <c r="Q35">
+        <v>11.264699999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" s="8"/>
+      <c r="I36">
+        <v>15.731999999999999</v>
+      </c>
+      <c r="J36">
+        <v>15.112299999999999</v>
+      </c>
+      <c r="K36">
+        <v>12.0024</v>
+      </c>
+      <c r="O36">
+        <v>15.731999999999999</v>
+      </c>
+      <c r="P36">
+        <v>15.112299999999999</v>
+      </c>
+      <c r="Q36">
+        <v>12.0024</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>0.32679999999999998</v>
+      </c>
+      <c r="J38">
+        <v>0.38840000000000002</v>
+      </c>
+      <c r="K38">
+        <v>0.3916</v>
+      </c>
+      <c r="O38">
+        <v>0.32679999999999998</v>
+      </c>
+      <c r="P38">
+        <v>0.38840000000000002</v>
+      </c>
+      <c r="Q38">
+        <v>0.3916</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="J39">
+        <v>0.35220000000000001</v>
+      </c>
+      <c r="K39">
+        <v>0.36080000000000001</v>
+      </c>
+      <c r="O39">
+        <v>0.30180000000000001</v>
+      </c>
+      <c r="P39">
+        <v>0.35220000000000001</v>
+      </c>
+      <c r="Q39">
+        <v>0.36080000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>0.2535</v>
+      </c>
+      <c r="J40">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="K40">
+        <v>0.30669999999999997</v>
+      </c>
+      <c r="O40">
+        <v>0.2535</v>
+      </c>
+      <c r="P40">
+        <v>0.30230000000000001</v>
+      </c>
+      <c r="Q40">
+        <v>0.30669999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>0.2316</v>
+      </c>
+      <c r="J41">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="K41">
+        <v>0.25109999999999999</v>
+      </c>
+      <c r="O41">
+        <v>0.2316</v>
+      </c>
+      <c r="P41">
+        <v>0.18870000000000001</v>
+      </c>
+      <c r="Q41">
+        <v>0.25109999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I2" t="s">
+        <v>276</v>
+      </c>
+      <c r="J2" t="s">
+        <v>274</v>
+      </c>
+      <c r="K2" t="s">
+        <v>202</v>
+      </c>
+      <c r="L2" t="s">
+        <v>275</v>
+      </c>
+      <c r="M2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.47776999999999997</v>
+      </c>
+      <c r="C4" s="10">
+        <v>13.364493</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.36004599999999998</v>
+      </c>
+      <c r="E4" s="11">
+        <v>0.73416000000000003</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0.48800300000000002</v>
+      </c>
+      <c r="G4" s="10">
+        <v>13.069471</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.37370399999999998</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.72708399999999995</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.59818199999999999</v>
+      </c>
+      <c r="K4" s="10">
+        <v>9.2014779999999998</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.50383299999999998</v>
+      </c>
+      <c r="M4" s="11">
+        <v>0.82509600000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10">
+        <v>12.9682</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.38150000000000001</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0.72230000000000005</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="10">
+        <v>12.484999999999999</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0.40110000000000001</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.72989999999999999</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10">
+        <v>8.8089999999999993</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.52549999999999997</v>
+      </c>
+      <c r="M5" s="11">
+        <v>0.81489999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10">
+        <v>13.5182</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.3478</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0.72519999999999996</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="10">
+        <v>13.2623</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0.35780000000000001</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.72150000000000003</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10">
+        <v>9.3857999999999997</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0.49070000000000003</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0.81499999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10">
+        <v>15.301399999999999</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.2742</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0.68010000000000004</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="10">
+        <v>16.097000000000001</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.26700000000000002</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.6653</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10">
+        <v>11.007099999999999</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0.42059999999999997</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0.77649999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13">
+        <v>17.459399999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <v>0.2306</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.61660000000000004</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13">
+        <v>18.9833</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0.21729999999999999</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13">
+        <v>12.4541</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0.3306</v>
+      </c>
+      <c r="M8" s="14">
+        <v>0.64780000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>252</v>
+      </c>
+      <c r="J11" t="s">
+        <v>252</v>
+      </c>
+      <c r="S11" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B12">
+        <v>0.65085700000000002</v>
+      </c>
+      <c r="C12">
+        <v>7.8736639999999998</v>
+      </c>
+      <c r="D12">
+        <v>0.52854199999999996</v>
+      </c>
+      <c r="E12">
+        <v>0.85342099999999999</v>
+      </c>
+      <c r="J12" t="s">
+        <v>258</v>
+      </c>
+      <c r="T12" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>270</v>
+      </c>
+      <c r="C13">
+        <v>7.4871999999999996</v>
+      </c>
+      <c r="D13">
+        <v>0.53920000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.8125</v>
+      </c>
+      <c r="J13" t="s">
+        <v>259</v>
+      </c>
+      <c r="S13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C14">
+        <v>8.8543000000000003</v>
+      </c>
+      <c r="D14">
+        <v>0.4985</v>
+      </c>
+      <c r="E14">
+        <v>0.79820000000000002</v>
+      </c>
+      <c r="J14" t="s">
+        <v>260</v>
+      </c>
+      <c r="S14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>272</v>
+      </c>
+      <c r="C15">
+        <v>11.5494</v>
+      </c>
+      <c r="D15">
+        <v>0.46310000000000001</v>
+      </c>
+      <c r="E15">
+        <v>0.79920000000000002</v>
+      </c>
+      <c r="J15" t="s">
+        <v>261</v>
+      </c>
+      <c r="S15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>253</v>
+      </c>
+      <c r="J18" t="s">
+        <v>253</v>
+      </c>
+      <c r="S18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0.74116300000000002</v>
+      </c>
+      <c r="C19">
+        <v>5.5367649999999999</v>
+      </c>
+      <c r="D19">
+        <v>0.57670999999999994</v>
+      </c>
+      <c r="E19">
+        <v>0.94171400000000005</v>
+      </c>
+      <c r="K19" t="s">
+        <v>254</v>
+      </c>
+      <c r="T19" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>5.4706000000000001</v>
+      </c>
+      <c r="D20">
+        <v>0.58069999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.94589999999999996</v>
+      </c>
+      <c r="J20" t="s">
+        <v>255</v>
+      </c>
+      <c r="S20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>6.4592999999999998</v>
+      </c>
+      <c r="D21">
+        <v>0.5202</v>
+      </c>
+      <c r="E21">
+        <v>0.88300000000000001</v>
+      </c>
+      <c r="J21" t="s">
+        <v>256</v>
+      </c>
+      <c r="S21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>8.9869000000000003</v>
+      </c>
+      <c r="D22">
+        <v>0.44069999999999998</v>
+      </c>
+      <c r="E22">
+        <v>0.71189999999999998</v>
+      </c>
+      <c r="J22" t="s">
+        <v>257</v>
+      </c>
+      <c r="S22" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>6.4721000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L33">
+        <v>7.2714999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L34">
+        <v>8.7472999999999992</v>
+      </c>
+    </row>
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L35">
+        <v>9.9297000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:R24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>253</v>
+      </c>
+      <c r="H2" t="s">
+        <v>252</v>
+      </c>
+      <c r="N2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E3" t="s">
+        <v>284</v>
+      </c>
+      <c r="I3" t="s">
+        <v>281</v>
+      </c>
+      <c r="J3" t="s">
+        <v>282</v>
+      </c>
+      <c r="K3" t="s">
+        <v>283</v>
+      </c>
+      <c r="L3" t="s">
+        <v>284</v>
+      </c>
+      <c r="O3" t="s">
+        <v>281</v>
+      </c>
+      <c r="P3" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>283</v>
+      </c>
+      <c r="R3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>285</v>
+      </c>
+      <c r="H4" t="s">
+        <v>289</v>
+      </c>
+      <c r="N4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>286</v>
+      </c>
+      <c r="H5" t="s">
+        <v>290</v>
+      </c>
+      <c r="N5" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H6" t="s">
+        <v>291</v>
+      </c>
+      <c r="N6" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>288</v>
+      </c>
+      <c r="H7" t="s">
+        <v>292</v>
+      </c>
+      <c r="N7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>253</v>
+      </c>
+      <c r="H10" t="s">
+        <v>252</v>
+      </c>
+      <c r="N10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" t="s">
+        <v>282</v>
+      </c>
+      <c r="D11" t="s">
+        <v>283</v>
+      </c>
+      <c r="E11" t="s">
+        <v>284</v>
+      </c>
+      <c r="I11" t="s">
+        <v>281</v>
+      </c>
+      <c r="J11" t="s">
+        <v>282</v>
+      </c>
+      <c r="K11" t="s">
+        <v>283</v>
+      </c>
+      <c r="L11" t="s">
+        <v>284</v>
+      </c>
+      <c r="O11" t="s">
+        <v>281</v>
+      </c>
+      <c r="P11" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>283</v>
+      </c>
+      <c r="R11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>298</v>
+      </c>
+      <c r="H12" t="s">
+        <v>302</v>
+      </c>
+      <c r="N12" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>299</v>
+      </c>
+      <c r="H13" t="s">
+        <v>303</v>
+      </c>
+      <c r="N13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>300</v>
+      </c>
+      <c r="H14" t="s">
+        <v>304</v>
+      </c>
+      <c r="N14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>301</v>
+      </c>
+      <c r="H15" t="s">
+        <v>305</v>
+      </c>
+      <c r="N15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>253</v>
+      </c>
+      <c r="H18" t="s">
+        <v>252</v>
+      </c>
+      <c r="N18" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" t="s">
+        <v>283</v>
+      </c>
+      <c r="E19" t="s">
+        <v>284</v>
+      </c>
+      <c r="I19" t="s">
+        <v>281</v>
+      </c>
+      <c r="J19" t="s">
+        <v>282</v>
+      </c>
+      <c r="K19" t="s">
+        <v>283</v>
+      </c>
+      <c r="L19" t="s">
+        <v>284</v>
+      </c>
+      <c r="O19" t="s">
+        <v>281</v>
+      </c>
+      <c r="P19" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>283</v>
+      </c>
+      <c r="R19" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>311</v>
+      </c>
+      <c r="H20" t="s">
+        <v>315</v>
+      </c>
+      <c r="N20" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>312</v>
+      </c>
+      <c r="H21" t="s">
+        <v>316</v>
+      </c>
+      <c r="N21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>313</v>
+      </c>
+      <c r="H22" t="s">
+        <v>317</v>
+      </c>
+      <c r="N22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>314</v>
+      </c>
+      <c r="H23" t="s">
+        <v>318</v>
+      </c>
+      <c r="N23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:AI48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O16" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>324</v>
+      </c>
+      <c r="K4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E6" t="s">
+        <v>282</v>
+      </c>
+      <c r="F6" t="s">
+        <v>283</v>
+      </c>
+      <c r="G6" t="s">
+        <v>284</v>
+      </c>
+      <c r="K6" t="s">
+        <v>340</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>326</v>
+      </c>
+      <c r="K8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>17</v>
+      </c>
+      <c r="X8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>327</v>
+      </c>
+      <c r="K9" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>324</v>
+      </c>
+      <c r="X9" t="s">
+        <v>324</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="10" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>328</v>
+      </c>
+      <c r="K10" t="s">
+        <v>342</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>253</v>
+      </c>
+      <c r="X10" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>252</v>
+      </c>
+      <c r="R11" t="s">
+        <v>281</v>
+      </c>
+      <c r="S11" t="s">
+        <v>282</v>
+      </c>
+      <c r="T11" t="s">
+        <v>283</v>
+      </c>
+      <c r="U11" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>281</v>
+      </c>
+      <c r="M12" t="s">
+        <v>282</v>
+      </c>
+      <c r="N12" t="s">
+        <v>283</v>
+      </c>
+      <c r="O12" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>351</v>
+      </c>
+      <c r="X12" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="13" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>329</v>
+      </c>
+      <c r="K13" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>352</v>
+      </c>
+      <c r="X13" t="s">
+        <v>360</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>344</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>353</v>
+      </c>
+      <c r="X14" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="15" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>330</v>
+      </c>
+      <c r="K15" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>354</v>
+      </c>
+      <c r="X15" t="s">
+        <v>362</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>346</v>
+      </c>
+      <c r="X16" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>324</v>
+      </c>
+      <c r="K23" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>17</v>
+      </c>
+      <c r="X23" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>252</v>
+      </c>
+      <c r="K24" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>324</v>
+      </c>
+      <c r="X24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>281</v>
+      </c>
+      <c r="E25" t="s">
+        <v>282</v>
+      </c>
+      <c r="F25" t="s">
+        <v>283</v>
+      </c>
+      <c r="G25" t="s">
+        <v>284</v>
+      </c>
+      <c r="K25" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>253</v>
+      </c>
+      <c r="X25" t="s">
+        <v>251</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>331</v>
+      </c>
+      <c r="L26" t="s">
+        <v>281</v>
+      </c>
+      <c r="M26" t="s">
+        <v>282</v>
+      </c>
+      <c r="N26" t="s">
+        <v>283</v>
+      </c>
+      <c r="O26" t="s">
+        <v>284</v>
+      </c>
+      <c r="R26" t="s">
+        <v>281</v>
+      </c>
+      <c r="S26" t="s">
+        <v>282</v>
+      </c>
+      <c r="T26" t="s">
+        <v>283</v>
+      </c>
+      <c r="U26" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>332</v>
+      </c>
+      <c r="K27" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>355</v>
+      </c>
+      <c r="X27" t="s">
+        <v>364</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>333</v>
+      </c>
+      <c r="K28" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>356</v>
+      </c>
+      <c r="X28" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH28" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI28" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>334</v>
+      </c>
+      <c r="K29" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>357</v>
+      </c>
+      <c r="X29" t="s">
+        <v>366</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>350</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>358</v>
+      </c>
+      <c r="X30" t="s">
+        <v>367</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="X31" t="s">
+        <v>368</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>17</v>
+      </c>
+      <c r="X37" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="K38" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>324</v>
+      </c>
+      <c r="X38" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>253</v>
+      </c>
+      <c r="X39" t="s">
+        <v>251</v>
+      </c>
+      <c r="AE39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="L40" t="s">
+        <v>281</v>
+      </c>
+      <c r="M40" t="s">
+        <v>282</v>
+      </c>
+      <c r="N40" t="s">
+        <v>283</v>
+      </c>
+      <c r="O40" t="s">
+        <v>284</v>
+      </c>
+      <c r="R40" t="s">
+        <v>281</v>
+      </c>
+      <c r="S40" t="s">
+        <v>282</v>
+      </c>
+      <c r="T40" t="s">
+        <v>283</v>
+      </c>
+      <c r="U40" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>282</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>283</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>284</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>24</v>
+      </c>
+      <c r="K41" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>373</v>
+      </c>
+      <c r="X41" t="s">
+        <v>377</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>324</v>
+      </c>
+      <c r="K42" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>374</v>
+      </c>
+      <c r="X42" t="s">
+        <v>378</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG42" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH42" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI42" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>252</v>
+      </c>
+      <c r="K43" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>375</v>
+      </c>
+      <c r="X43" t="s">
+        <v>379</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>281</v>
+      </c>
+      <c r="E44" t="s">
+        <v>282</v>
+      </c>
+      <c r="F44" t="s">
+        <v>283</v>
+      </c>
+      <c r="G44" t="s">
+        <v>284</v>
+      </c>
+      <c r="K44" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>376</v>
+      </c>
+      <c r="X44" t="s">
+        <v>380</v>
+      </c>
+      <c r="AE44" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>336</v>
+      </c>
+      <c r="X45" t="s">
+        <v>381</v>
+      </c>
+      <c r="AE45" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE46" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
age and gender experiment better organized
</commit_message>
<xml_diff>
--- a/age_gender/performance.xlsx
+++ b/age_gender/performance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="5880" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="15600" windowHeight="5880" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="402">
   <si>
     <t>FGNET</t>
   </si>
@@ -1201,6 +1202,30 @@
   </si>
   <si>
     <t xml:space="preserve">   10.5405    0.3140    0.8322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.2434    0.3702    0.8618</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.2323    0.3724    0.8577</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.1661    0.3736    0.8698</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9.7745    0.3330    0.8465</t>
+  </si>
+  <si>
+    <t>Yamaha lambda eval</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>gender acc</t>
+  </si>
+  <si>
+    <t>age acc</t>
   </si>
 </sst>
 </file>
@@ -1346,7 +1371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1390,6 +1415,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4853,10 +4879,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:AI48"/>
+  <dimension ref="C4:AI55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O16" workbookViewId="0">
-      <selection activeCell="AF34" sqref="AF34"/>
+    <sheetView topLeftCell="T37" workbookViewId="0">
+      <selection activeCell="AF48" sqref="AF48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5542,6 +5568,151 @@
         <v>339</v>
       </c>
     </row>
+    <row r="50" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AE50" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="51" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AF51" t="s">
+        <v>281</v>
+      </c>
+      <c r="AG51" t="s">
+        <v>282</v>
+      </c>
+      <c r="AH51" t="s">
+        <v>283</v>
+      </c>
+      <c r="AI51" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="52" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AE52" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="53" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AE53" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="54" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AE54" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="55" spans="31:35" x14ac:dyDescent="0.25">
+      <c r="AE55" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>20.714600000000001</v>
+      </c>
+      <c r="C3">
+        <v>0.1341</v>
+      </c>
+      <c r="D3">
+        <v>0.49109999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>1E-3</v>
+      </c>
+      <c r="B4">
+        <v>7.7108999999999996</v>
+      </c>
+      <c r="C4">
+        <v>0.4173</v>
+      </c>
+      <c r="D4">
+        <v>0.92169999999999996</v>
+      </c>
+      <c r="F4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="21"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>1.9999999999999999E-6</v>
+      </c>
+      <c r="F8" s="21"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B9">
+        <v>7.0058999999999996</v>
+      </c>
+      <c r="C9">
+        <v>0.46539999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.92220000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>